<commit_message>
Se agregan cambios en estructura de vista y controladores, se valida crud en los modulos.
</commit_message>
<xml_diff>
--- a/progreso.xlsx
+++ b/progreso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
   <si>
     <t>Asociados</t>
   </si>
@@ -118,13 +118,97 @@
   </si>
   <si>
     <t>Cambios</t>
+  </si>
+  <si>
+    <t>Se modifica interfaz, de acuerdo a los modulos.</t>
+  </si>
+  <si>
+    <t>Se ajusta modulo de autenticacion de acuerdo a la accesibilidad de los modulos.</t>
+  </si>
+  <si>
+    <t>* Permite ver  * No edita * no elimina * permite agregar</t>
+  </si>
+  <si>
+    <t>Tipos_identificaciones</t>
+  </si>
+  <si>
+    <t>* CRUD - permite C-R-U-D</t>
+  </si>
+  <si>
+    <t>Generos</t>
+  </si>
+  <si>
+    <t>Validar campo id, tiene limite a un a un caracter</t>
+  </si>
+  <si>
+    <t>EstadosP</t>
+  </si>
+  <si>
+    <t>Permite ver y crear, no actualiza ni elimina</t>
+  </si>
+  <si>
+    <t>Tipos_Asoc</t>
+  </si>
+  <si>
+    <t>Tipos_Drog</t>
+  </si>
+  <si>
+    <t>Campo codigo: ¿Cambiar a varchar? Solo acepta numeros</t>
+  </si>
+  <si>
+    <t>Campo identificacion: ¿Cambiar a varchar? Solo acepta numeros</t>
+  </si>
+  <si>
+    <t>Droguerias_P</t>
+  </si>
+  <si>
+    <t>Tabla muestra solo los datos de foreing_key, cambiarlo para mostrar los datos mas legible</t>
+  </si>
+  <si>
+    <t>Departamentos</t>
+  </si>
+  <si>
+    <t>Ciudades</t>
+  </si>
+  <si>
+    <t>* Permite ver  * No edita * permite eliminar * permite agregar</t>
+  </si>
+  <si>
+    <t>Indicativos_ciu</t>
+  </si>
+  <si>
+    <t>¿Cambiar por indicativos_paises?</t>
+  </si>
+  <si>
+    <t>Modulos</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Se ajusta estructura de vistas y controladores en funcion de los modulos</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +216,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -168,11 +272,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -181,13 +282,37 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -485,11 +610,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -509,278 +634,278 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -788,49 +913,359 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="43.453125" style="4" customWidth="1"/>
+    <col min="1" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>45400</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>45390</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>45417</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
+      <c r="B15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="12"/>
+      <c r="B23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="12"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="13">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:A26"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>